<commit_message>
Fixes + registrykey feature
- The infrastructure of tests reworks so we could test some new features, like the introduction of the registrykeycheck function that is part of the sprint 2
- Some errors identified in sprint 1 have been fixed
</commit_message>
<xml_diff>
--- a/Documentations/JDT_NRO.xlsx
+++ b/Documentations/JDT_NRO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eduvaud-my.sharepoint.com/personal/pf32wyn_eduvaud_ch/Documents/Documents/New Git/WSRVCHECKER/Documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="339" documentId="13_ncr:1_{5DE8A0A8-6501-4ECA-8318-9CDF0F24E7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{579B58F6-9647-471F-8AB0-749DD5652567}"/>
+  <xr:revisionPtr revIDLastSave="466" documentId="13_ncr:1_{5DE8A0A8-6501-4ECA-8318-9CDF0F24E7DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C6BE97F-0190-49CD-9B17-6CAFDF6960E6}"/>
   <bookViews>
-    <workbookView xWindow="9705" yWindow="3180" windowWidth="18300" windowHeight="9345" xr2:uid="{86DB9306-B773-4C37-83F0-F8CCD26E2979}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{86DB9306-B773-4C37-83F0-F8CCD26E2979}"/>
   </bookViews>
   <sheets>
     <sheet name="JDT" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="102">
   <si>
     <t>Date</t>
   </si>
@@ -308,6 +308,42 @@
   <si>
     <t>Certaines lignes s'écrivent en double</t>
   </si>
+  <si>
+    <t>Tentative de correction du problème sur le serveur membre du domaine</t>
+  </si>
+  <si>
+    <t>Le serveur n'arrive pas à accèder à l'Active Directory ( aucune manipulation n'a été effectuée, les machines ont été allumés et une erreur apparaît quand nous voulons accéder à l'AD )</t>
+  </si>
+  <si>
+    <t>Même problème que au dessus, même après "l'aide" de M. Yawo et Varella, aucune solution pour l'instant</t>
+  </si>
+  <si>
+    <t>Tentative de correction du problème sur un des serveurs membre du domaine</t>
+  </si>
+  <si>
+    <t>Meeting avec M. Glassey</t>
+  </si>
+  <si>
+    <t>Travail sur le nouveau sprint ( RegistryKey )</t>
+  </si>
+  <si>
+    <t>Après discussion avec M. Glassey, on a décidé de se concentrer sur les nouveautés plutôt que les correctifs afin d'avoir un livrable et pouvoir valider avec JBU jeudi durant notre meeting</t>
+  </si>
+  <si>
+    <t>Réunion avec M. Glassey et les autres élèves sous lui afin de discuter du TPI/la suite</t>
+  </si>
+  <si>
+    <t>Pourcentages</t>
+  </si>
+  <si>
+    <t>Réparation d'une partie importante du script et revue globale pour mettre au point l'avancée</t>
+  </si>
+  <si>
+    <t>J'ai fait un recap d'où en est le script car après le changement de serveurs et les problèmes que j'ai rencontré, j'ai perdu quelques petites améliorations que j'avais effectué et donc une partie du script ne fonctionnait plus car ancienne version de tests récuperée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le script est capable d'aller chercher et lire la clé de registre cépendant je n'ai pas encore pu faire les fonctions pour les potentiels résultats, je pense que j'arriverai à commencer quelques unes Jeudi matin avant la réunion avec JBU et M. Glassey </t>
+  </si>
 </sst>
 </file>
 
@@ -389,7 +425,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -410,15 +446,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -476,12 +503,54 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color theme="0"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="0"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
       <bottom style="thin">
         <color theme="0"/>
       </bottom>
@@ -492,7 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -512,31 +581,52 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -854,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26502E31-8F11-4A1D-87B5-02A720D7DBAA}">
-  <dimension ref="B1:H1359"/>
+  <dimension ref="B1:N1359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,43 +959,50 @@
     <col min="5" max="6" width="19.42578125" style="4" customWidth="1"/>
     <col min="7" max="7" width="92.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="57" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
+    <col min="9" max="10" width="11.42578125" style="2"/>
+    <col min="11" max="11" width="22.7109375" style="2" customWidth="1"/>
+    <col min="12" max="13" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="17.28515625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="K1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="14" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="N1" s="11"/>
+    </row>
+    <row r="2" spans="2:14" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="12"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="K2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11" t="s">
+      <c r="L2" s="19"/>
+      <c r="M2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="8">
-        <f>SUM(E5:E495)</f>
-        <v>2.6041666666666652</v>
-      </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="N2" s="19"/>
+    </row>
+    <row r="3" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -913,8 +1010,14 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K3" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,8 +1039,15 @@
       <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K4" s="15">
+        <f>SUM(E5:E495)</f>
+        <v>3.1215277777777759</v>
+      </c>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="16"/>
+    </row>
+    <row r="5" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>45323</v>
       </c>
@@ -960,8 +1070,14 @@
       <c r="H5" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="K5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+    </row>
+    <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>45323</v>
       </c>
@@ -984,8 +1100,16 @@
       <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>45323</v>
       </c>
@@ -1005,8 +1129,12 @@
       <c r="G7" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>45323</v>
       </c>
@@ -1029,8 +1157,16 @@
       <c r="H8" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K8" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="M8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>45323</v>
       </c>
@@ -1050,8 +1186,12 @@
       <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>45323</v>
       </c>
@@ -1072,7 +1212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>45323</v>
       </c>
@@ -1096,7 +1236,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>45324</v>
       </c>
@@ -1120,7 +1260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>45324</v>
       </c>
@@ -1141,7 +1281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>45324</v>
       </c>
@@ -1162,7 +1302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>45328</v>
       </c>
@@ -1183,7 +1323,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>45328</v>
       </c>
@@ -2362,58 +2502,211 @@
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B71" s="3">
+        <v>45365</v>
+      </c>
+      <c r="C71" s="6">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D71" s="6">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E71" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B72" s="3">
+        <v>45365</v>
+      </c>
+      <c r="C72" s="6">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="D72" s="6">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="E72" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+        <v>0.10069444444444436</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B73" s="3">
+        <v>45365</v>
+      </c>
+      <c r="C73" s="6">
+        <v>0.5625</v>
+      </c>
+      <c r="D73" s="6">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="E73" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.14236111111111116</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="3">
+        <v>45366</v>
+      </c>
+      <c r="C74" s="6">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D74" s="6">
+        <v>0.5</v>
+      </c>
       <c r="E74" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.9027777777777735E-2</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C75" s="6">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D75" s="6">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="E75" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B76" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C76" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D76" s="6">
+        <v>0.4375</v>
+      </c>
       <c r="E76" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B77" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C77" s="6">
+        <v>0.4375</v>
+      </c>
+      <c r="D77" s="6">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="E77" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C78" s="6">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D78" s="6">
+        <v>0.50694444444444442</v>
+      </c>
       <c r="E78" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B79" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C79" s="6">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D79" s="6">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="E79" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.7777777777777679E-2</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
@@ -10098,12 +10391,23 @@
     </row>
   </sheetData>
   <autoFilter ref="B4:H1359" xr:uid="{26502E31-8F11-4A1D-87B5-02A720D7DBAA}"/>
-  <mergeCells count="5">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="G1:H2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
+  <mergeCells count="16">
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B1:H2"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>